<commit_message>
Integrated some extern applications
-fixed a few tcp errors and incosistencies
-fixed dmx output
-fixed wifi qrcode
-updated gui
</commit_message>
<xml_diff>
--- a/Spa_Interaction_Screen_Content/ConfigFile.xlsx
+++ b/Spa_Interaction_Screen_Content/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berni\Documents\GitHub\Spa_Interaction_Screen\Spa_Interaction_Screen_Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{713E7426-7C8A-4850-84FE-E05C984043D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{848E677E-4C18-4C73-9E26-CDDD082E2B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2745" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="260" uniqueCount="170">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="263" uniqueCount="170">
   <si>
     <t>default</t>
   </si>
@@ -68,9 +68,6 @@
     <t>frische Handtücher</t>
   </si>
   <si>
-    <t>Arzt</t>
-  </si>
-  <si>
     <t>Putzlicht</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>#(Connecting to Port 80/443)</t>
   </si>
   <si>
-    <t>DMXScenes</t>
-  </si>
-  <si>
     <t>#(Wird nur im Service Tab angezeigt)</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>#Order Importance</t>
   </si>
   <si>
-    <t>#(Wird nur angezeigt, wenn nicht 0) (Wird in der Laufzeit bearbeitet)</t>
-  </si>
-  <si>
     <t>#Dimmer1 Channel</t>
   </si>
   <si>
@@ -323,9 +314,6 @@
     <t>#Arduino Com Port Name</t>
   </si>
   <si>
-    <t>#CH0</t>
-  </si>
-  <si>
     <t>Was kann ich heute für Sie tun?</t>
   </si>
   <si>
@@ -549,6 +537,18 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>Scenes</t>
+  </si>
+  <si>
+    <t>#1 based</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Aufguss</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q72" sqref="Q72"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,42 +1036,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" s="14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -1079,10 +1082,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>192</v>
@@ -1099,10 +1102,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5">
         <v>8000</v>
@@ -1110,10 +1113,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C6">
         <v>5004</v>
@@ -1121,43 +1124,43 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>666</v>
@@ -1165,10 +1168,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1191,35 +1194,35 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>192</v>
@@ -1236,10 +1239,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>23</v>
@@ -1247,24 +1250,24 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -1272,98 +1275,98 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" t="s">
         <v>127</v>
       </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18" t="s">
         <v>128</v>
-      </c>
-      <c r="F18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" t="s">
-        <v>131</v>
-      </c>
-      <c r="I18" t="s">
-        <v>133</v>
-      </c>
-      <c r="J18" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1371,19 +1374,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1391,51 +1394,51 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D28">
         <v>15</v>
@@ -1443,87 +1446,87 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1534,16 +1537,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1554,16 +1557,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C35">
         <v>7</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E35">
         <v>9</v>
@@ -1574,84 +1577,84 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D36" s="13"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D42" s="13">
         <v>0</v>
@@ -1660,13 +1663,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <v>15</v>
@@ -1675,30 +1678,30 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1706,13 +1709,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -1720,151 +1723,151 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C50">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F52" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="F55" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" t="s">
-        <v>95</v>
-      </c>
-      <c r="F55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1872,41 +1875,33 @@
       <c r="D56" t="s">
         <v>7</v>
       </c>
-      <c r="E56" t="str">
-        <f xml:space="preserve">  B48 &amp; "," &amp; C50 &amp; "," &amp; "true,true, false"</f>
-        <v>Session,15,true,true, false</v>
-      </c>
       <c r="F56" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" t="s">
+        <v>169</v>
+      </c>
+      <c r="F57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="str">
-        <f xml:space="preserve">  B60 &amp; "," &amp; C62 &amp; "," &amp; "true,true, false"</f>
-        <v>DMXScenes,Putzlicht,true,true, false</v>
-      </c>
-      <c r="F57" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -1914,58 +1909,54 @@
       <c r="D58" t="s">
         <v>8</v>
       </c>
-      <c r="E58" t="str">
-        <f xml:space="preserve">  B54 &amp; "," &amp; C57 &amp; "," &amp; "true,true, false"</f>
-        <v>Services,Notfall,true,true, false</v>
-      </c>
       <c r="F58" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>26</v>
@@ -1974,57 +1965,57 @@
         <v>27</v>
       </c>
       <c r="O60" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P60" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="R60" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="S60" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T60" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P60" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q60" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="R60" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S60" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="T60" s="6" t="s">
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="U60" s="4" t="s">
+      <c r="B61" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" t="s">
-        <v>30</v>
-      </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="E61">
+        <v>255</v>
       </c>
       <c r="F61">
-        <v>255</v>
+        <v>56</v>
       </c>
       <c r="G61">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="J61">
         <v>128</v>
       </c>
       <c r="K61">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>255</v>
@@ -2047,37 +2038,34 @@
       <c r="R61">
         <v>0</v>
       </c>
-      <c r="S61">
-        <v>0</v>
-      </c>
-      <c r="T61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F62">
+        <v>200</v>
+      </c>
+      <c r="G62">
+        <v>128</v>
+      </c>
+      <c r="H62">
         <v>255</v>
-      </c>
-      <c r="G62">
-        <v>200</v>
-      </c>
-      <c r="H62">
-        <v>128</v>
       </c>
       <c r="I62">
         <v>255</v>
@@ -2086,10 +2074,10 @@
         <v>255</v>
       </c>
       <c r="K62">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="L62">
-        <v>255</v>
+        <v>100</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -2109,263 +2097,307 @@
       <c r="R62">
         <v>0</v>
       </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-      <c r="U62" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63">
+        <v>255</v>
+      </c>
+      <c r="F63">
+        <v>200</v>
+      </c>
+      <c r="G63">
+        <v>128</v>
+      </c>
+      <c r="H63">
+        <v>255</v>
+      </c>
+      <c r="I63">
+        <v>255</v>
+      </c>
+      <c r="J63">
+        <v>255</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>255</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>100</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
         <v>24</v>
       </c>
-      <c r="C63" t="s">
-        <v>84</v>
-      </c>
-      <c r="D63" t="s">
-        <v>165</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <v>0</v>
-      </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="O63">
+      <c r="C64" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" t="s">
+        <v>161</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65">
         <v>255</v>
       </c>
-      <c r="P63">
-        <v>0</v>
-      </c>
-      <c r="Q63">
-        <v>0</v>
-      </c>
-      <c r="R63">
-        <v>0</v>
-      </c>
-      <c r="S63">
-        <v>0</v>
-      </c>
-      <c r="U63" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
         <v>255</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
         <v>255</v>
       </c>
-      <c r="M64">
-        <v>0</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="O64">
-        <v>0</v>
-      </c>
-      <c r="P64">
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
         <v>255</v>
       </c>
-      <c r="Q64">
-        <v>0</v>
-      </c>
-      <c r="R64">
-        <v>0</v>
-      </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
-      <c r="T64" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>35</v>
-      </c>
-      <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
         <v>255</v>
       </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-      <c r="M65">
-        <v>0</v>
-      </c>
-      <c r="N65">
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
         <v>255</v>
       </c>
-      <c r="O65">
-        <v>0</v>
-      </c>
-      <c r="P65">
-        <v>0</v>
-      </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
-      <c r="R65">
-        <v>0</v>
-      </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>35</v>
-      </c>
-      <c r="B66" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>128</v>
+      </c>
+      <c r="J67">
+        <v>128</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
         <v>255</v>
       </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
-      <c r="J66">
-        <v>128</v>
-      </c>
-      <c r="K66">
-        <v>128</v>
-      </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-      <c r="M66">
-        <v>255</v>
-      </c>
-      <c r="P66">
-        <v>0</v>
-      </c>
-      <c r="Q66">
-        <v>0</v>
-      </c>
-      <c r="R66">
-        <v>0</v>
-      </c>
-      <c r="S66">
-        <v>0</v>
-      </c>
-      <c r="T66" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>55</v>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>